<commit_message>
xcel updated success as pass and added name as tom
</commit_message>
<xml_diff>
--- a/SalesTool/data/Zoho.xlsx
+++ b/SalesTool/data/Zoho.xlsx
@@ -93,9 +93,6 @@
     <t>Lenovo</t>
   </si>
   <si>
-    <t>Sam</t>
-  </si>
-  <si>
     <t>Watson</t>
   </si>
   <si>
@@ -138,10 +135,13 @@
     <t>rajshahlive@gmail.com</t>
   </si>
   <si>
-    <t>Success</t>
-  </si>
-  <si>
-    <t>No_Success</t>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Tom</t>
   </si>
 </sst>
 </file>
@@ -603,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -647,13 +647,13 @@
         <v>14</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" t="s">
         <v>39</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -670,7 +670,7 @@
         <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -717,7 +717,7 @@
         <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -731,7 +731,7 @@
         <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -745,7 +745,7 @@
         <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -775,10 +775,10 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" t="s">
         <v>28</v>
-      </c>
-      <c r="D15" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -794,16 +794,16 @@
         <v>10</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -814,16 +814,16 @@
         <v>14</v>
       </c>
       <c r="C19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D19" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="F19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>